<commit_message>
Content update and modification to release process to maintain a modified date
</commit_message>
<xml_diff>
--- a/xlsx/Old/funders.xlsx
+++ b/xlsx/Old/funders.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emckclac-my.sharepoint.com/personal/k1780970_kcl_ac_uk/Documents/1. Catalogue + work documents/1. Catalogue shared files/1. Catalogue/2. Catalogue study updates/Funders files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{0F7304FC-427B-7E49-A9EE-3A29E7B8DC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0A80414-EC47-408A-9DD5-30DAACE29B3B}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{0F7304FC-427B-7E49-A9EE-3A29E7B8DC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A753856B-049F-45CD-886A-AB0283C7E2E9}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="0" windowWidth="21000" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="236">
   <si>
     <t>Logos saved</t>
   </si>
@@ -370,7 +371,7 @@
     <t>MRC</t>
   </si>
   <si>
-    <t>https://mrc.ukri.org/</t>
+    <t>https://www.ukri.org/councils/mrc/</t>
   </si>
   <si>
     <t>Ministry of Justice</t>
@@ -487,6 +488,15 @@
     <t>https://www.nuffieldfoundation.org/</t>
   </si>
   <si>
+    <t>Office for Veterans' Affairs</t>
+  </si>
+  <si>
+    <t>OfVA</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/organisations/office-for-veterans-affairs</t>
+  </si>
+  <si>
     <t>ONS</t>
   </si>
   <si>
@@ -641,6 +651,15 @@
   </si>
   <si>
     <t>https://www.uq.edu.au/</t>
+  </si>
+  <si>
+    <t>University of Southampton</t>
+  </si>
+  <si>
+    <t>SOTON</t>
+  </si>
+  <si>
+    <t>https://www.southampton.ac.uk/</t>
   </si>
   <si>
     <t>US Department of Health and Human Services</t>
@@ -836,10 +855,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1223,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="172" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="172" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -1242,11 +1261,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1350,7 +1369,7 @@
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1650,7 +1669,7 @@
       <c r="B36" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1797,58 +1816,58 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" ht="15">
       <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="C50" s="9" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" s="6" t="s">
+      <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="B51" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="A52" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="B52" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15">
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" ht="15">
       <c r="A54" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="11" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1892,29 +1911,29 @@
       <c r="B58" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15">
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="10" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" ht="15">
       <c r="A60" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="11" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1936,7 +1955,7 @@
       <c r="B62" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="4" t="s">
         <v>184</v>
       </c>
     </row>
@@ -1947,7 +1966,7 @@
       <c r="B63" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="5" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1962,25 +1981,25 @@
         <v>190</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15">
+    <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" ht="15">
       <c r="A66" s="1" t="s">
         <v>194</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="9" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2006,14 +2025,14 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" ht="15">
       <c r="A69" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="11" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2029,54 +2048,54 @@
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="4" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="7" customFormat="1" ht="15">
-      <c r="A73" s="8" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" s="7" t="s">
         <v>215</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="5" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:3" s="7" customFormat="1" ht="15">
+      <c r="A75" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="7" t="s">
         <v>222</v>
       </c>
       <c r="C75" s="9" t="s">
@@ -2105,16 +2124,38 @@
         <v>229</v>
       </c>
     </row>
+    <row r="78" spans="1:3" ht="15">
+      <c r="A78" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15">
+      <c r="A79" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C70">
-    <sortCondition ref="A3:A70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C72">
+    <sortCondition ref="A3:A72"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C61" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C62" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="C11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
@@ -2128,13 +2169,13 @@
     <hyperlink ref="C19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="C21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="C22" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C68" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C70" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="C23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C66" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C67" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="C26" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="C24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="C29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C63" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C64" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="C31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="C33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="C37" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
@@ -2146,42 +2187,44 @@
     <hyperlink ref="C44" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
     <hyperlink ref="C39" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="C46" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C50" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C52" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C54" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C57" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C56" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C53" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C55" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C58" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C57" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
     <hyperlink ref="C15" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C67" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C60" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C69" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C70" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C64" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C68" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C61" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C71" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C72" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C65" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
     <hyperlink ref="C41" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
     <hyperlink ref="C35" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
     <hyperlink ref="C48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C62" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C63" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="C5" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
     <hyperlink ref="C38" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
     <hyperlink ref="C49" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C71" r:id="rId52" xr:uid="{D4EC3F26-FB9B-0C4C-A9BF-D5766209B760}"/>
-    <hyperlink ref="C72" r:id="rId53" xr:uid="{4FBF0906-9AF5-D142-B9D1-1BEF3B0A1FEE}"/>
-    <hyperlink ref="C73" r:id="rId54" xr:uid="{0D9565FC-23CE-7743-ADFA-9A087B7C25D3}"/>
-    <hyperlink ref="C74" r:id="rId55" xr:uid="{47453487-DE29-E249-95B5-E46513555F55}"/>
-    <hyperlink ref="C75" r:id="rId56" xr:uid="{D034833B-B5AE-614C-B976-B8F12F8AB280}"/>
-    <hyperlink ref="C76" r:id="rId57" xr:uid="{D069C9A5-D5AC-0B46-A34E-B50258C56053}"/>
-    <hyperlink ref="C77" r:id="rId58" xr:uid="{BE3AC031-8C70-9C41-8DC7-88700E8C32CA}"/>
-    <hyperlink ref="C65" r:id="rId59" xr:uid="{DF192853-BCD5-E947-A105-44BE7CB5CF72}"/>
+    <hyperlink ref="C73" r:id="rId52" xr:uid="{D4EC3F26-FB9B-0C4C-A9BF-D5766209B760}"/>
+    <hyperlink ref="C74" r:id="rId53" xr:uid="{4FBF0906-9AF5-D142-B9D1-1BEF3B0A1FEE}"/>
+    <hyperlink ref="C75" r:id="rId54" xr:uid="{0D9565FC-23CE-7743-ADFA-9A087B7C25D3}"/>
+    <hyperlink ref="C76" r:id="rId55" xr:uid="{47453487-DE29-E249-95B5-E46513555F55}"/>
+    <hyperlink ref="C77" r:id="rId56" xr:uid="{D034833B-B5AE-614C-B976-B8F12F8AB280}"/>
+    <hyperlink ref="C78" r:id="rId57" xr:uid="{D069C9A5-D5AC-0B46-A34E-B50258C56053}"/>
+    <hyperlink ref="C79" r:id="rId58" xr:uid="{BE3AC031-8C70-9C41-8DC7-88700E8C32CA}"/>
+    <hyperlink ref="C66" r:id="rId59" xr:uid="{DF192853-BCD5-E947-A105-44BE7CB5CF72}"/>
     <hyperlink ref="C7" r:id="rId60" xr:uid="{470CBD7E-33DA-4B21-B8E2-B4245DC824F9}"/>
     <hyperlink ref="C32" r:id="rId61" xr:uid="{6D3F7EC2-6E99-4830-BFBD-AF4938F90032}"/>
     <hyperlink ref="C34" r:id="rId62" xr:uid="{A5049810-F177-4DB3-8129-6A0BCC790164}"/>
     <hyperlink ref="C8" r:id="rId63" xr:uid="{AC0D0AB7-0BC3-4F09-BDD1-2E7C15FC0C4F}"/>
-    <hyperlink ref="C58" r:id="rId64" xr:uid="{5259C5DB-4130-4B45-97CA-D23E8CE07F78}"/>
-    <hyperlink ref="C53" r:id="rId65" xr:uid="{A61A251B-14DB-4690-AC31-7A1836680CF3}"/>
-    <hyperlink ref="C59" r:id="rId66" xr:uid="{58614A08-2023-451C-9C66-88C2FD08E9AE}"/>
+    <hyperlink ref="C59" r:id="rId64" xr:uid="{5259C5DB-4130-4B45-97CA-D23E8CE07F78}"/>
+    <hyperlink ref="C54" r:id="rId65" xr:uid="{A61A251B-14DB-4690-AC31-7A1836680CF3}"/>
+    <hyperlink ref="C60" r:id="rId66" xr:uid="{58614A08-2023-451C-9C66-88C2FD08E9AE}"/>
     <hyperlink ref="C9" r:id="rId67" xr:uid="{A374CCDF-5F4A-4B09-B50F-80F234168E91}"/>
+    <hyperlink ref="C50" r:id="rId68" xr:uid="{941F840C-1B87-4863-A9DA-679DE419CC00}"/>
+    <hyperlink ref="C69" r:id="rId69" xr:uid="{3A7EB2C3-4F2B-4CBC-BB56-FE1E9592C8AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId68"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId70"/>
 </worksheet>
 </file>
</xml_diff>